<commit_message>
added the variables in js file
</commit_message>
<xml_diff>
--- a/files/Tip calculator app.xlsx
+++ b/files/Tip calculator app.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00. RMA\_TECNOLOGIA\mentoria-pedroMarins\tip-calculator-app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E3DCAB-4425-4070-84ED-65AB3D68F5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591E81E1-0E45-4EDC-82BC-E3679FB6B2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{700BB218-8BE2-42CC-9C26-601D4E0290D4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>tip per person</t>
   </si>
@@ -60,14 +60,26 @@
     <t>prompt</t>
   </si>
   <si>
-    <t>todos os botões</t>
+    <t>tip-custom</t>
+  </si>
+  <si>
+    <t>button reset</t>
+  </si>
+  <si>
+    <t>error message</t>
+  </si>
+  <si>
+    <t>CALCULAR E MOSTRAR</t>
+  </si>
+  <si>
+    <t>CAPTURAR, innerhtml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +91,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -131,6 +150,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,39 +467,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E7CBF9-C44D-4353-BD48-E429597FCC25}">
-  <dimension ref="C4:G16"/>
+  <dimension ref="C2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="2"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D4">
         <v>142.55000000000001</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1</v>
+      </c>
       <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="1">
@@ -486,73 +540,146 @@
       <c r="F7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="D10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9">
-        <f>D6*D7</f>
+      <c r="D12">
+        <f>D4*D7</f>
         <v>21.3825</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="H12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11">
-        <f>D6+D9</f>
+      <c r="D14">
+        <f>D4+D12</f>
         <v>163.9325</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="H14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+      <c r="H16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="4">
-        <f>D9/D13</f>
+      <c r="D18" s="4">
+        <f>D12/D16</f>
         <v>4.2765000000000004</v>
       </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="4">
-        <f>D11/D13</f>
+      <c r="D19" s="4">
+        <f>D14/D16</f>
         <v>32.786500000000004</v>
       </c>
-      <c r="F16" t="s">
-        <v>9</v>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>